<commit_message>
Update 2021 HWL2 First Batch
</commit_message>
<xml_diff>
--- a/rebuild/IndicPriorityList.xlsx
+++ b/rebuild/IndicPriorityList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IndicatorsPriority" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="142">
   <si>
     <t xml:space="preserve">IndicatorsList</t>
   </si>
@@ -57,12 +57,79 @@
     <t xml:space="preserve">Life Expectancy &lt;br&gt; at Birth (Total)</t>
   </si>
   <si>
+    <t xml:space="preserve">Global Extreme Poverty Cost of Basic Needs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Global Extreme </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;br&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Poverty Cost of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;br&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Basic Needs</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Extreme Poverty (CBN)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Height</t>
   </si>
   <si>
     <t xml:space="preserve">Income Inequality</t>
   </si>
   <si>
+    <t xml:space="preserve">Wealth Yearly Ginis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wealth Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wealth Top10 percent share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wealth Decadal Ginis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Numeracy (Total)</t>
   </si>
   <si>
@@ -121,6 +188,52 @@
   </si>
   <si>
     <t xml:space="preserve">Male life Expectancy &lt;br&gt; at Birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Extreme Poverty Dollar a Day </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Global Extreme </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;br&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Poverty Dollar </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;br&gt; a Day</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Extreme Poverty (DAD)</t>
   </si>
   <si>
     <t xml:space="preserve">Height Gini</t>
@@ -499,8 +612,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -508,42 +629,37 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="B81:B84 E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.1015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.219387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.4030612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.10204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,69 +762,69 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>8</v>
@@ -717,18 +833,18 @@
         <v>0</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>9</v>
@@ -737,18 +853,18 @@
         <v>1</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>10</v>
@@ -757,18 +873,18 @@
         <v>0</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>11</v>
@@ -777,13 +893,13 @@
         <v>0</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -797,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>20</v>
@@ -808,27 +924,27 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>14</v>
@@ -837,58 +953,58 @@
         <v>1</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>15</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>17</v>
@@ -897,18 +1013,18 @@
         <v>1</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>18</v>
@@ -917,58 +1033,58 @@
         <v>1</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>19</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>21</v>
@@ -977,18 +1093,18 @@
         <v>1</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>22</v>
@@ -997,18 +1113,18 @@
         <v>1</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>23</v>
@@ -1017,78 +1133,78 @@
         <v>1</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>25</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>26</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>27</v>
@@ -1097,13 +1213,13 @@
         <v>1</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>49</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1120,7 +1236,7 @@
         <v>51</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>50</v>
@@ -1128,7 +1244,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>29</v>
@@ -1137,18 +1253,18 @@
         <v>1</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>30</v>
@@ -1157,18 +1273,18 @@
         <v>1</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>31</v>
@@ -1177,13 +1293,13 @@
         <v>1</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>57</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,10 +1353,10 @@
         <v>1</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>60</v>
@@ -1248,7 +1364,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>35</v>
@@ -1257,18 +1373,18 @@
         <v>1</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>36</v>
@@ -1277,18 +1393,18 @@
         <v>1</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>37</v>
@@ -1297,18 +1413,18 @@
         <v>1</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>38</v>
@@ -1317,18 +1433,18 @@
         <v>1</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>39</v>
@@ -1337,18 +1453,18 @@
         <v>1</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>40</v>
@@ -1357,18 +1473,18 @@
         <v>1</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>41</v>
@@ -1377,18 +1493,18 @@
         <v>1</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>42</v>
@@ -1397,18 +1513,18 @@
         <v>1</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>43</v>
@@ -1417,18 +1533,18 @@
         <v>1</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>44</v>
@@ -1437,18 +1553,18 @@
         <v>1</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>45</v>
@@ -1460,10 +1576,10 @@
         <v>75</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,13 +1590,13 @@
         <v>46</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>76</v>
@@ -1488,67 +1604,67 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>47</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>48</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>49</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>50</v>
@@ -1557,18 +1673,18 @@
         <v>1</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>51</v>
@@ -1577,98 +1693,98 @@
         <v>1</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>52</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>87</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>53</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>54</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>55</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>56</v>
@@ -1677,18 +1793,18 @@
         <v>1</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>57</v>
@@ -1697,18 +1813,18 @@
         <v>1</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>58</v>
@@ -1717,18 +1833,18 @@
         <v>1</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>59</v>
@@ -1737,18 +1853,18 @@
         <v>1</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>60</v>
@@ -1757,18 +1873,18 @@
         <v>1</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>61</v>
@@ -1777,98 +1893,98 @@
         <v>1</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>62</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>63</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>64</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>65</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>66</v>
@@ -1877,18 +1993,18 @@
         <v>1</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>67</v>
@@ -1900,55 +2016,55 @@
         <v>106</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>68</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>69</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>70</v>
@@ -1957,159 +2073,279 @@
         <v>0</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>71</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>72</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>73</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>74</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>75</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D76" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E76" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="E76" s="0" t="s">
-        <v>123</v>
-      </c>
       <c r="F76" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>76</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E77" s="0" t="s">
         <v>124</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>77</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D78" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="E78" s="0" t="s">
+      <c r="B79" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="E79" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="F78" s="0" t="s">
-        <v>126</v>
+      <c r="F79" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2118,21 +2354,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B81:B84 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2140,7 +2374,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2148,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2156,13 +2390,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2171,26 +2405,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B81" activeCellId="0" sqref="B81:B84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>131</v>
+      <c r="A1" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
@@ -2198,146 +2431,146 @@
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,90 +2583,90 @@
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2446,42 +2679,42 @@
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2494,250 +2727,250 @@
     </row>
     <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2750,72 +2983,120 @@
     </row>
     <row r="71" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>